<commit_message>
Removed a phantom "App1" from XAML source
Also updated XLSX file.
</commit_message>
<xml_diff>
--- a/blogPosts/Article Resources and Links.xlsx
+++ b/blogPosts/Article Resources and Links.xlsx
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Day</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>http://msdn.microsoft.com/en-us/library/windows/apps/hh465319.aspx</t>
+  </si>
+  <si>
+    <t>http://csell.net/2012/11/01/31-days-of-windows-8-day-1-the-blank-app</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added new Day #5 article and code (incomplete)
</commit_message>
<xml_diff>
--- a/blogPosts/Article Resources and Links.xlsx
+++ b/blogPosts/Article Resources and Links.xlsx
@@ -176,12 +176,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="F7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Settings Guidance</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Day</t>
   </si>
@@ -262,13 +286,16 @@
   </si>
   <si>
     <t>http://csell.net/2012/11/01/31-days-of-windows-8-day-1-the-blank-app</t>
+  </si>
+  <si>
+    <t>http://msdn.microsoft.com/en-us/library/windows/apps/hh770544.aspx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +321,19 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -631,7 +671,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +822,9 @@
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added day 1 to the site
</commit_message>
<xml_diff>
--- a/blogPosts/Article Resources and Links.xlsx
+++ b/blogPosts/Article Resources and Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Day</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>http://msdn.microsoft.com/en-us/library/windows/apps/hh770544.aspx</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/HTML5/Day1-TheBlankApp</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/HTML5/Day2-OrientationAndSnapping</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/HTML5/Day6-Search</t>
   </si>
 </sst>
 </file>
@@ -671,15 +680,17 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99" customWidth="1"/>
+    <col min="3" max="3" width="47.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,8 +750,8 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -760,8 +771,8 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
@@ -831,6 +842,9 @@
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -990,9 +1004,12 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B5" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="E3" r:id="rId6"/>
+    <hyperlink ref="E4" r:id="rId7"/>
+    <hyperlink ref="E8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId6"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Day #6 Article and Code (incomplete)
</commit_message>
<xml_diff>
--- a/blogPosts/Article Resources and Links.xlsx
+++ b/blogPosts/Article Resources and Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,12 +200,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="F8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+MSDN Search Guidance</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Day</t>
   </si>
@@ -258,9 +282,6 @@
     <t>XAML DL</t>
   </si>
   <si>
-    <t>http://bit.ly/31daysofwindows8-day1code</t>
-  </si>
-  <si>
     <t>http://msdn.microsoft.com/en-us/library/hh191443.aspx</t>
   </si>
   <si>
@@ -270,15 +291,9 @@
     <t>http://www.microsoft.com/en-us/download/details.aspx?id=30674</t>
   </si>
   <si>
-    <t>http://bit.ly/31daysofwindows8-day2code</t>
-  </si>
-  <si>
     <t>http://msdn.microsoft.com/en-us/library/windows/apps/windows.applicationmodel.activation.splashscreen.aspx</t>
   </si>
   <si>
-    <t>http://bit.ly/31daysofwindows8-day3code</t>
-  </si>
-  <si>
     <t>http://msdn.microsoft.com/library/windows/apps/BR227716</t>
   </si>
   <si>
@@ -298,6 +313,27 @@
   </si>
   <si>
     <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/HTML5/Day6-Search</t>
+  </si>
+  <si>
+    <t>http://msdn.microsoft.com/en-us/library/windows/apps/hh465233.aspx</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/XAML/Day1-TheBlankApp</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/XAML/Day2-OrientationAndSnap</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/XAML/Day3-SplashScreen</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/XAML/Day4-NewControls</t>
+  </si>
+  <si>
+    <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/XAML/Day5-SettingsContract</t>
+  </si>
+  <si>
+    <t>http://www.jeffblankenburg.com/2012/11/05/31-days-of-windows-8-day-5-settings-contract</t>
   </si>
 </sst>
 </file>
@@ -679,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,13 +781,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -769,19 +805,19 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -796,13 +832,13 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -817,16 +853,16 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -834,8 +870,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -844,7 +886,10 @@
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1007,9 +1052,10 @@
     <hyperlink ref="E3" r:id="rId6"/>
     <hyperlink ref="E4" r:id="rId7"/>
     <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="B7" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
locked up day #3 for the site
</commit_message>
<xml_diff>
--- a/blogPosts/Article Resources and Links.xlsx
+++ b/blogPosts/Article Resources and Links.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19632" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Day</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>https://github.com/csell5/31DaysOfWindows8/tree/master/source/HTML5/Day6-Search</t>
+  </si>
+  <si>
+    <t>http://csell.net/2012/11/03/31-days-of-windows-8-day-3-the-splash-screen/?preview=true&amp;preview_id=561</t>
   </si>
 </sst>
 </file>
@@ -679,22 +682,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="105.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="105.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -726,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -737,7 +740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>1</v>
@@ -758,7 +761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A33" si="0">A3+1</f>
         <v>2</v>
@@ -785,7 +788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -793,8 +796,8 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -806,7 +809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -830,7 +833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -839,7 +842,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -848,151 +851,151 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1008,9 +1011,10 @@
     <hyperlink ref="E3" r:id="rId6"/>
     <hyperlink ref="E4" r:id="rId7"/>
     <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1020,7 +1024,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1032,7 +1036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>